<commit_message>
Plan de pruebas parte 1 y 2
</commit_message>
<xml_diff>
--- a/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-1.xlsx
+++ b/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-1.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t xml:space="preserve">RESULTADO OBTENIDO </t>
   </si>
@@ -224,6 +224,9 @@
     <t>Personal médico</t>
   </si>
   <si>
+    <t>Médico</t>
+  </si>
+  <si>
     <t>CENTRO MÉDICO HIPÓCRATES</t>
   </si>
   <si>
@@ -279,6 +282,42 @@
   </si>
   <si>
     <t>Despliega mensaje adecuado.</t>
+  </si>
+  <si>
+    <t>Actualizar ficha medica</t>
+  </si>
+  <si>
+    <t>Se actualiza la ficha medica del paciente</t>
+  </si>
+  <si>
+    <t>Médico actualiza ficha medica</t>
+  </si>
+  <si>
+    <t>Médico intenta actualizar ficha médica del paciente con datos vacíos</t>
+  </si>
+  <si>
+    <t>Buscar paciente para actualizar ficha medica y no ingresar los datos requeridos</t>
+  </si>
+  <si>
+    <t>Buscar paciente para actualizar ficha medica y completar el formulario con los datos requeridos</t>
+  </si>
+  <si>
+    <t>Derivar consulta medica</t>
+  </si>
+  <si>
+    <t>Médico deriva una consulta medica</t>
+  </si>
+  <si>
+    <t>Médico intenta derivar una consulta medica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar paciente para derivar consulta medica y seleccionar datos específicos </t>
+  </si>
+  <si>
+    <t>Se deriva una consulta medica para el paciente</t>
+  </si>
+  <si>
+    <t>Buscar paciente para derivar consulta medica y no completar los datos requeridos</t>
   </si>
 </sst>
 </file>
@@ -500,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -526,6 +565,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -614,6 +654,22 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1122,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:M23"/>
+  <dimension ref="B5:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1205,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1167,7 +1223,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1185,7 +1241,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1202,290 +1258,353 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="17">
+      <c r="E9" s="18">
         <v>42703</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="21" t="s">
+      <c r="E11" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="16"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B12" s="25"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="12" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="26" t="s">
+      <c r="K12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="20">
         <v>1</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="2:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="20">
+        <v>2</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="2:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="20">
+        <v>3</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="G15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="29"/>
+    </row>
+    <row r="16" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="C16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="20">
+        <v>4</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="2:13" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="15" t="s">
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="20">
+        <v>5</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="2:13" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="19">
-        <v>3</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="15" t="s">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="2:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="B18" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="20">
+        <v>6</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="2:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="B16" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="19">
-        <v>4</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="15" t="s">
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="29"/>
+    </row>
+    <row r="19" spans="2:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="B19" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="20">
+        <v>7</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="27"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="19">
-        <v>5</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="19">
-        <v>6</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="28"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="27"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="19">
-        <v>7</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="28"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="27"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="19">
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="29"/>
+    </row>
+    <row r="20" spans="2:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="B20" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="20">
         <v>8</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="28"/>
+      <c r="E20" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="29"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="27"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="19">
-        <v>9</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="28"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="27"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="19">
-        <v>10</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="28"/>
-    </row>
-    <row r="23" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31">
-        <v>11</v>
-      </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="34"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="29"/>
+    </row>
+    <row r="22" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="35"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="36"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>